<commit_message>
Update Userstories and TDD Testcases For College Admission Predictor project modified.xlsx
</commit_message>
<xml_diff>
--- a/Userstories and TDD Testcases For College Admission Predictor project modified.xlsx
+++ b/Userstories and TDD Testcases For College Admission Predictor project modified.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kommahes\Documents\GitHub\-College-Admission-Predictor\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="6" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2 (2)" sheetId="5" state="hidden" r:id="rId1"/>
@@ -1145,15 +1150,9 @@
     <t>End Date</t>
   </si>
   <si>
-    <t>Yet To Start</t>
-  </si>
-  <si>
     <t>Yet to start</t>
   </si>
   <si>
-    <t>yet to start</t>
-  </si>
-  <si>
     <t>start Date</t>
   </si>
   <si>
@@ -1161,12 +1160,18 @@
   </si>
   <si>
     <t>2.5 Reset Password</t>
+  </si>
+  <si>
+    <t>WIP</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="35">
     <font>
       <sz val="11"/>
@@ -2588,6 +2593,15 @@
     <xf numFmtId="14" fontId="0" fillId="6" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2658,6 +2672,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2730,18 +2747,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3052,7 +3057,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3065,7 +3070,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3076,106 +3081,106 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" customWidth="1"/>
+    <col min="3" max="3" width="29.1796875" customWidth="1"/>
+    <col min="4" max="4" width="28.81640625" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
-    <col min="6" max="6" width="40.85546875" customWidth="1"/>
-    <col min="7" max="7" width="40.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
-    <col min="10" max="11" width="17.5703125" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="40.81640625" customWidth="1"/>
+    <col min="7" max="7" width="40.1796875" customWidth="1"/>
+    <col min="8" max="8" width="16.1796875" customWidth="1"/>
+    <col min="9" max="9" width="18.1796875" customWidth="1"/>
+    <col min="10" max="11" width="17.54296875" customWidth="1"/>
+    <col min="12" max="12" width="18.54296875" customWidth="1"/>
     <col min="13" max="13" width="24" customWidth="1"/>
-    <col min="14" max="14" width="21.85546875" customWidth="1"/>
+    <col min="14" max="14" width="21.81640625" customWidth="1"/>
     <col min="15" max="15" width="49" customWidth="1"/>
-    <col min="16" max="16" width="57.5703125" customWidth="1"/>
+    <col min="16" max="16" width="57.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="176" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="175" t="s">
+      <c r="B1" s="178" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
-      <c r="O1" s="175"/>
-      <c r="P1" s="175"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+      <c r="H1" s="178"/>
+      <c r="I1" s="178"/>
+      <c r="J1" s="178"/>
+      <c r="K1" s="178"/>
+      <c r="L1" s="178"/>
+      <c r="M1" s="178"/>
+      <c r="N1" s="178"/>
+      <c r="O1" s="178"/>
+      <c r="P1" s="178"/>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="174"/>
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
-      <c r="I2" s="175"/>
-      <c r="J2" s="175"/>
-      <c r="K2" s="175"/>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175"/>
-      <c r="N2" s="175"/>
-      <c r="O2" s="175"/>
-      <c r="P2" s="175"/>
+      <c r="A2" s="177"/>
+      <c r="B2" s="178"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="178"/>
+      <c r="I2" s="178"/>
+      <c r="J2" s="178"/>
+      <c r="K2" s="178"/>
+      <c r="L2" s="178"/>
+      <c r="M2" s="178"/>
+      <c r="N2" s="178"/>
+      <c r="O2" s="178"/>
+      <c r="P2" s="178"/>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="174"/>
-      <c r="B3" s="176"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
-      <c r="F3" s="176"/>
-      <c r="G3" s="176"/>
-      <c r="H3" s="176"/>
-      <c r="I3" s="176"/>
-      <c r="J3" s="176"/>
-      <c r="K3" s="176"/>
-      <c r="L3" s="176"/>
-      <c r="M3" s="176"/>
-      <c r="N3" s="176"/>
-      <c r="O3" s="176"/>
-      <c r="P3" s="176"/>
-    </row>
-    <row r="4" spans="1:16" ht="26.25">
+      <c r="A3" s="177"/>
+      <c r="B3" s="179"/>
+      <c r="C3" s="179"/>
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="179"/>
+      <c r="H3" s="179"/>
+      <c r="I3" s="179"/>
+      <c r="J3" s="179"/>
+      <c r="K3" s="179"/>
+      <c r="L3" s="179"/>
+      <c r="M3" s="179"/>
+      <c r="N3" s="179"/>
+      <c r="O3" s="179"/>
+      <c r="P3" s="179"/>
+    </row>
+    <row r="4" spans="1:16" ht="26">
       <c r="A4" s="13"/>
-      <c r="B4" s="177" t="s">
+      <c r="B4" s="180" t="s">
         <v>263</v>
       </c>
-      <c r="C4" s="177"/>
-      <c r="D4" s="177"/>
-      <c r="E4" s="177"/>
-      <c r="F4" s="177"/>
-      <c r="G4" s="177"/>
-      <c r="H4" s="177"/>
-      <c r="I4" s="177"/>
-      <c r="J4" s="177"/>
-      <c r="K4" s="177"/>
-      <c r="L4" s="177"/>
-      <c r="M4" s="177"/>
-      <c r="N4" s="177"/>
-      <c r="O4" s="177"/>
-      <c r="P4" s="178"/>
+      <c r="C4" s="180"/>
+      <c r="D4" s="180"/>
+      <c r="E4" s="180"/>
+      <c r="F4" s="180"/>
+      <c r="G4" s="180"/>
+      <c r="H4" s="180"/>
+      <c r="I4" s="180"/>
+      <c r="J4" s="180"/>
+      <c r="K4" s="180"/>
+      <c r="L4" s="180"/>
+      <c r="M4" s="180"/>
+      <c r="N4" s="180"/>
+      <c r="O4" s="180"/>
+      <c r="P4" s="181"/>
     </row>
     <row r="5" spans="1:16" ht="60.75" customHeight="1">
       <c r="A5" s="14"/>
@@ -3225,8 +3230,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="96.6" customHeight="1">
-      <c r="A6" s="179" t="s">
+    <row r="6" spans="1:16" ht="96.65" customHeight="1">
+      <c r="A6" s="182" t="s">
         <v>242</v>
       </c>
       <c r="B6" s="33" t="s">
@@ -3255,7 +3260,7 @@
         <v>43977</v>
       </c>
       <c r="K6" s="36" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="L6" s="154">
         <v>43979</v>
@@ -3270,7 +3275,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="66.75" customHeight="1">
-      <c r="A7" s="180"/>
+      <c r="A7" s="183"/>
       <c r="B7" s="33" t="s">
         <v>102</v>
       </c>
@@ -3297,7 +3302,7 @@
         <v>43979</v>
       </c>
       <c r="K7" s="36" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="L7" s="154">
         <v>43980</v>
@@ -3314,7 +3319,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="63" customHeight="1">
-      <c r="A8" s="180"/>
+      <c r="A8" s="183"/>
       <c r="B8" s="33" t="s">
         <v>102</v>
       </c>
@@ -3341,7 +3346,7 @@
         <v>43980</v>
       </c>
       <c r="K8" s="36" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="L8" s="154">
         <v>43983</v>
@@ -3371,41 +3376,41 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:BY137"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="30" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" style="29" customWidth="1"/>
-    <col min="4" max="13" width="33.42578125" style="29" customWidth="1"/>
-    <col min="14" max="14" width="61.5703125" style="31" customWidth="1"/>
-    <col min="15" max="15" width="68.7109375" style="12" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="32.7265625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="21.81640625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="30.1796875" style="29" customWidth="1"/>
+    <col min="4" max="13" width="33.453125" style="29" customWidth="1"/>
+    <col min="14" max="14" width="61.54296875" style="31" customWidth="1"/>
+    <col min="15" max="15" width="68.7265625" style="12" customWidth="1"/>
+    <col min="16" max="16384" width="9.1796875" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:77" ht="15" customHeight="1">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="176" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="175" t="s">
+      <c r="B1" s="178" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
-      <c r="O1" s="175"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+      <c r="H1" s="178"/>
+      <c r="I1" s="178"/>
+      <c r="J1" s="178"/>
+      <c r="K1" s="178"/>
+      <c r="L1" s="178"/>
+      <c r="M1" s="178"/>
+      <c r="N1" s="178"/>
+      <c r="O1" s="178"/>
       <c r="P1" s="10"/>
       <c r="Q1" s="10"/>
       <c r="R1" s="10"/>
@@ -3470,21 +3475,21 @@
       <c r="BY1" s="11"/>
     </row>
     <row r="2" spans="1:77" ht="15" customHeight="1">
-      <c r="A2" s="174"/>
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
-      <c r="I2" s="175"/>
-      <c r="J2" s="175"/>
-      <c r="K2" s="175"/>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175"/>
-      <c r="N2" s="175"/>
-      <c r="O2" s="175"/>
+      <c r="A2" s="177"/>
+      <c r="B2" s="178"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="178"/>
+      <c r="I2" s="178"/>
+      <c r="J2" s="178"/>
+      <c r="K2" s="178"/>
+      <c r="L2" s="178"/>
+      <c r="M2" s="178"/>
+      <c r="N2" s="178"/>
+      <c r="O2" s="178"/>
       <c r="P2" s="10"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="10"/>
@@ -3549,21 +3554,21 @@
       <c r="BY2" s="11"/>
     </row>
     <row r="3" spans="1:77" ht="15" customHeight="1">
-      <c r="A3" s="174"/>
-      <c r="B3" s="176"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
-      <c r="F3" s="176"/>
-      <c r="G3" s="176"/>
-      <c r="H3" s="176"/>
-      <c r="I3" s="176"/>
-      <c r="J3" s="176"/>
-      <c r="K3" s="176"/>
-      <c r="L3" s="176"/>
-      <c r="M3" s="176"/>
-      <c r="N3" s="176"/>
-      <c r="O3" s="176"/>
+      <c r="A3" s="177"/>
+      <c r="B3" s="179"/>
+      <c r="C3" s="179"/>
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="179"/>
+      <c r="H3" s="179"/>
+      <c r="I3" s="179"/>
+      <c r="J3" s="179"/>
+      <c r="K3" s="179"/>
+      <c r="L3" s="179"/>
+      <c r="M3" s="179"/>
+      <c r="N3" s="179"/>
+      <c r="O3" s="179"/>
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
@@ -3627,22 +3632,22 @@
       <c r="BX3" s="11"/>
       <c r="BY3" s="11"/>
     </row>
-    <row r="4" spans="1:77" ht="26.25">
+    <row r="4" spans="1:77" ht="26">
       <c r="A4" s="13"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="177"/>
-      <c r="D4" s="177"/>
-      <c r="E4" s="177"/>
-      <c r="F4" s="177"/>
-      <c r="G4" s="177"/>
-      <c r="H4" s="177"/>
-      <c r="I4" s="177"/>
-      <c r="J4" s="177"/>
-      <c r="K4" s="177"/>
-      <c r="L4" s="177"/>
-      <c r="M4" s="177"/>
-      <c r="N4" s="177"/>
-      <c r="O4" s="178"/>
+      <c r="B4" s="180"/>
+      <c r="C4" s="180"/>
+      <c r="D4" s="180"/>
+      <c r="E4" s="180"/>
+      <c r="F4" s="180"/>
+      <c r="G4" s="180"/>
+      <c r="H4" s="180"/>
+      <c r="I4" s="180"/>
+      <c r="J4" s="180"/>
+      <c r="K4" s="180"/>
+      <c r="L4" s="180"/>
+      <c r="M4" s="180"/>
+      <c r="N4" s="180"/>
+      <c r="O4" s="181"/>
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
@@ -3814,7 +3819,7 @@
       <c r="BY5" s="11"/>
     </row>
     <row r="6" spans="1:77" ht="45" customHeight="1">
-      <c r="A6" s="181" t="s">
+      <c r="A6" s="184" t="s">
         <v>200</v>
       </c>
       <c r="B6" s="95" t="s">
@@ -3916,8 +3921,8 @@
       <c r="BX6" s="11"/>
       <c r="BY6" s="11"/>
     </row>
-    <row r="7" spans="1:77" ht="45">
-      <c r="A7" s="181"/>
+    <row r="7" spans="1:77" ht="43.5">
+      <c r="A7" s="184"/>
       <c r="B7" s="95" t="s">
         <v>37</v>
       </c>
@@ -4017,8 +4022,8 @@
       <c r="BX7" s="11"/>
       <c r="BY7" s="11"/>
     </row>
-    <row r="8" spans="1:77" ht="45">
-      <c r="A8" s="181"/>
+    <row r="8" spans="1:77" ht="43.5">
+      <c r="A8" s="184"/>
       <c r="B8" s="95" t="s">
         <v>102</v>
       </c>
@@ -4117,8 +4122,8 @@
       <c r="BX8" s="11"/>
       <c r="BY8" s="11"/>
     </row>
-    <row r="9" spans="1:77" ht="45">
-      <c r="A9" s="181"/>
+    <row r="9" spans="1:77" ht="43.5">
+      <c r="A9" s="184"/>
       <c r="B9" s="95" t="s">
         <v>37</v>
       </c>
@@ -4217,8 +4222,8 @@
       <c r="BX9" s="11"/>
       <c r="BY9" s="11"/>
     </row>
-    <row r="10" spans="1:77" ht="45">
-      <c r="A10" s="182"/>
+    <row r="10" spans="1:77" ht="29">
+      <c r="A10" s="185"/>
       <c r="B10" s="95" t="s">
         <v>37</v>
       </c>
@@ -4318,7 +4323,7 @@
       <c r="BY10" s="11"/>
     </row>
     <row r="11" spans="1:77" ht="45" customHeight="1">
-      <c r="A11" s="179" t="s">
+      <c r="A11" s="182" t="s">
         <v>60</v>
       </c>
       <c r="B11" s="33" t="s">
@@ -4419,8 +4424,8 @@
       <c r="BX11" s="11"/>
       <c r="BY11" s="11"/>
     </row>
-    <row r="12" spans="1:77" ht="45">
-      <c r="A12" s="180"/>
+    <row r="12" spans="1:77" ht="43.5">
+      <c r="A12" s="183"/>
       <c r="B12" s="33" t="s">
         <v>37</v>
       </c>
@@ -4519,8 +4524,8 @@
       <c r="BX12" s="11"/>
       <c r="BY12" s="11"/>
     </row>
-    <row r="13" spans="1:77" ht="45">
-      <c r="A13" s="180"/>
+    <row r="13" spans="1:77" ht="43.5">
+      <c r="A13" s="183"/>
       <c r="B13" s="33" t="s">
         <v>102</v>
       </c>
@@ -4547,7 +4552,7 @@
       <c r="K13" s="153">
         <v>43980</v>
       </c>
-      <c r="L13" s="184" t="s">
+      <c r="L13" s="187" t="s">
         <v>233</v>
       </c>
       <c r="N13" s="22" t="s">
@@ -4619,8 +4624,8 @@
       <c r="BX13" s="11"/>
       <c r="BY13" s="11"/>
     </row>
-    <row r="14" spans="1:77" ht="60">
-      <c r="A14" s="183"/>
+    <row r="14" spans="1:77" ht="43.5">
+      <c r="A14" s="186"/>
       <c r="B14" s="97" t="s">
         <v>102</v>
       </c>
@@ -4647,7 +4652,7 @@
       <c r="K14" s="160">
         <v>43979</v>
       </c>
-      <c r="L14" s="214"/>
+      <c r="L14" s="188"/>
       <c r="N14" s="100" t="s">
         <v>240</v>
       </c>
@@ -4718,10 +4723,10 @@
       <c r="BY14" s="11"/>
     </row>
     <row r="15" spans="1:77" ht="80.25" customHeight="1">
-      <c r="A15" s="211"/>
+      <c r="A15" s="161"/>
       <c r="B15" s="103"/>
       <c r="C15" s="29" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>122</v>
@@ -4745,10 +4750,10 @@
         <v>233</v>
       </c>
       <c r="M15" s="105"/>
-      <c r="N15" s="212" t="s">
+      <c r="N15" s="162" t="s">
         <v>126</v>
       </c>
-      <c r="O15" s="213" t="s">
+      <c r="O15" s="163" t="s">
         <v>127</v>
       </c>
       <c r="P15" s="11"/>
@@ -4814,7 +4819,7 @@
       <c r="BX15" s="11"/>
       <c r="BY15" s="11"/>
     </row>
-    <row r="16" spans="1:77" ht="78.75">
+    <row r="16" spans="1:77" ht="78">
       <c r="A16" s="102" t="s">
         <v>242</v>
       </c>
@@ -4915,7 +4920,7 @@
       <c r="BX16" s="11"/>
       <c r="BY16" s="11"/>
     </row>
-    <row r="17" spans="1:77" ht="45">
+    <row r="17" spans="1:77" ht="43.5">
       <c r="A17" s="108"/>
       <c r="B17" s="109" t="s">
         <v>102</v>
@@ -5014,7 +5019,7 @@
       <c r="BX17" s="11"/>
       <c r="BY17" s="11"/>
     </row>
-    <row r="18" spans="1:77" ht="26.25">
+    <row r="18" spans="1:77" ht="26">
       <c r="A18" s="108"/>
       <c r="B18" s="109"/>
       <c r="C18" s="110"/>
@@ -5093,7 +5098,7 @@
       <c r="BX18" s="11"/>
       <c r="BY18" s="11"/>
     </row>
-    <row r="19" spans="1:77" ht="45">
+    <row r="19" spans="1:77" ht="29">
       <c r="A19" s="151"/>
       <c r="B19" s="103" t="s">
         <v>102</v>
@@ -5189,7 +5194,7 @@
       <c r="BX19" s="11"/>
       <c r="BY19" s="11"/>
     </row>
-    <row r="20" spans="1:77" ht="45">
+    <row r="20" spans="1:77" ht="43.5">
       <c r="A20" s="150"/>
       <c r="B20" s="103" t="s">
         <v>257</v>
@@ -5887,7 +5892,7 @@
       <c r="N37" s="28"/>
       <c r="O37" s="11"/>
     </row>
-    <row r="38" spans="1:15" ht="409.6">
+    <row r="38" spans="1:15">
       <c r="A38" s="27"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -7602,107 +7607,107 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="25.26953125" customWidth="1"/>
+    <col min="2" max="2" width="23.7265625" customWidth="1"/>
+    <col min="3" max="3" width="20.7265625" customWidth="1"/>
+    <col min="4" max="4" width="23.54296875" customWidth="1"/>
+    <col min="5" max="5" width="21.81640625" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
-    <col min="11" max="12" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" customWidth="1"/>
-    <col min="14" max="14" width="22.42578125" customWidth="1"/>
-    <col min="15" max="15" width="60.140625" customWidth="1"/>
-    <col min="16" max="16" width="59.85546875" customWidth="1"/>
+    <col min="7" max="7" width="31.453125" customWidth="1"/>
+    <col min="8" max="8" width="20.81640625" customWidth="1"/>
+    <col min="9" max="9" width="18.81640625" customWidth="1"/>
+    <col min="10" max="10" width="13.26953125" customWidth="1"/>
+    <col min="11" max="12" width="12.81640625" customWidth="1"/>
+    <col min="13" max="13" width="21.1796875" customWidth="1"/>
+    <col min="14" max="14" width="22.453125" customWidth="1"/>
+    <col min="15" max="15" width="60.1796875" customWidth="1"/>
+    <col min="16" max="16" width="59.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="176" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="175" t="s">
+      <c r="B1" s="178" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
-      <c r="O1" s="175"/>
-      <c r="P1" s="175"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+      <c r="H1" s="178"/>
+      <c r="I1" s="178"/>
+      <c r="J1" s="178"/>
+      <c r="K1" s="178"/>
+      <c r="L1" s="178"/>
+      <c r="M1" s="178"/>
+      <c r="N1" s="178"/>
+      <c r="O1" s="178"/>
+      <c r="P1" s="178"/>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="174"/>
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
-      <c r="I2" s="175"/>
-      <c r="J2" s="175"/>
-      <c r="K2" s="175"/>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175"/>
-      <c r="N2" s="175"/>
-      <c r="O2" s="175"/>
-      <c r="P2" s="175"/>
+      <c r="A2" s="177"/>
+      <c r="B2" s="178"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="178"/>
+      <c r="I2" s="178"/>
+      <c r="J2" s="178"/>
+      <c r="K2" s="178"/>
+      <c r="L2" s="178"/>
+      <c r="M2" s="178"/>
+      <c r="N2" s="178"/>
+      <c r="O2" s="178"/>
+      <c r="P2" s="178"/>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="174"/>
-      <c r="B3" s="176"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
-      <c r="F3" s="176"/>
-      <c r="G3" s="176"/>
-      <c r="H3" s="176"/>
-      <c r="I3" s="176"/>
-      <c r="J3" s="176"/>
-      <c r="K3" s="176"/>
-      <c r="L3" s="176"/>
-      <c r="M3" s="176"/>
-      <c r="N3" s="176"/>
-      <c r="O3" s="176"/>
-      <c r="P3" s="176"/>
-    </row>
-    <row r="4" spans="1:16" ht="26.25">
+      <c r="A3" s="177"/>
+      <c r="B3" s="179"/>
+      <c r="C3" s="179"/>
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="179"/>
+      <c r="H3" s="179"/>
+      <c r="I3" s="179"/>
+      <c r="J3" s="179"/>
+      <c r="K3" s="179"/>
+      <c r="L3" s="179"/>
+      <c r="M3" s="179"/>
+      <c r="N3" s="179"/>
+      <c r="O3" s="179"/>
+      <c r="P3" s="179"/>
+    </row>
+    <row r="4" spans="1:16" ht="26">
       <c r="A4" s="13"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="177"/>
-      <c r="D4" s="177"/>
-      <c r="E4" s="177"/>
-      <c r="F4" s="177"/>
-      <c r="G4" s="177"/>
-      <c r="H4" s="177"/>
-      <c r="I4" s="177"/>
-      <c r="J4" s="177"/>
-      <c r="K4" s="177"/>
-      <c r="L4" s="177"/>
-      <c r="M4" s="177"/>
-      <c r="N4" s="177"/>
-      <c r="O4" s="177"/>
-      <c r="P4" s="178"/>
+      <c r="B4" s="180"/>
+      <c r="C4" s="180"/>
+      <c r="D4" s="180"/>
+      <c r="E4" s="180"/>
+      <c r="F4" s="180"/>
+      <c r="G4" s="180"/>
+      <c r="H4" s="180"/>
+      <c r="I4" s="180"/>
+      <c r="J4" s="180"/>
+      <c r="K4" s="180"/>
+      <c r="L4" s="180"/>
+      <c r="M4" s="180"/>
+      <c r="N4" s="180"/>
+      <c r="O4" s="180"/>
+      <c r="P4" s="181"/>
     </row>
     <row r="5" spans="1:16" ht="50.25" customHeight="1">
-      <c r="A5" s="180" t="s">
+      <c r="A5" s="183" t="s">
         <v>183</v>
       </c>
       <c r="B5" s="15" t="s">
@@ -7752,7 +7757,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="114" customHeight="1">
-      <c r="A6" s="180"/>
+      <c r="A6" s="183"/>
       <c r="B6" s="33" t="s">
         <v>184</v>
       </c>
@@ -7782,9 +7787,9 @@
         <v>43978</v>
       </c>
       <c r="L6" s="94" t="s">
-        <v>313</v>
-      </c>
-      <c r="M6" s="185" t="s">
+        <v>317</v>
+      </c>
+      <c r="M6" s="189" t="s">
         <v>190</v>
       </c>
       <c r="N6" s="19"/>
@@ -7796,7 +7801,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="120" customHeight="1">
-      <c r="A7" s="180"/>
+      <c r="A7" s="183"/>
       <c r="B7" s="33" t="s">
         <v>184</v>
       </c>
@@ -7826,9 +7831,9 @@
         <v>43980</v>
       </c>
       <c r="L7" s="94" t="s">
-        <v>313</v>
-      </c>
-      <c r="M7" s="186"/>
+        <v>316</v>
+      </c>
+      <c r="M7" s="190"/>
       <c r="N7" s="19"/>
       <c r="O7" s="22" t="s">
         <v>198</v>
@@ -7858,27 +7863,27 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.1796875" customWidth="1"/>
+    <col min="2" max="2" width="33.7265625" customWidth="1"/>
+    <col min="3" max="3" width="33.26953125" customWidth="1"/>
+    <col min="4" max="4" width="38.54296875" customWidth="1"/>
+    <col min="5" max="5" width="24.453125" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="37.5" customHeight="1">
-      <c r="A1" s="187" t="s">
+      <c r="A1" s="191" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="187"/>
-      <c r="C1" s="187"/>
-      <c r="D1" s="187"/>
-      <c r="E1" s="187"/>
-      <c r="F1" s="187"/>
-      <c r="G1" s="187"/>
+      <c r="B1" s="191"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
+      <c r="E1" s="191"/>
+      <c r="F1" s="191"/>
+      <c r="G1" s="191"/>
     </row>
     <row r="2" spans="1:7" ht="49.5" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -7988,27 +7993,27 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" customWidth="1"/>
-    <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="45.81640625" customWidth="1"/>
+    <col min="3" max="3" width="44.26953125" customWidth="1"/>
+    <col min="4" max="4" width="34.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.453125" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
-    <col min="7" max="7" width="32.85546875" customWidth="1"/>
+    <col min="7" max="7" width="32.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="43.5" customHeight="1">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="192" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="189"/>
-      <c r="C1" s="189"/>
-      <c r="D1" s="189"/>
-      <c r="E1" s="189"/>
-      <c r="F1" s="189"/>
-      <c r="G1" s="189"/>
+      <c r="B1" s="193"/>
+      <c r="C1" s="193"/>
+      <c r="D1" s="193"/>
+      <c r="E1" s="193"/>
+      <c r="F1" s="193"/>
+      <c r="G1" s="193"/>
     </row>
     <row r="2" spans="1:7" ht="34.5" customHeight="1">
       <c r="A2" s="58" t="s">
@@ -8205,63 +8210,63 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" style="53" customWidth="1"/>
-    <col min="2" max="3" width="19.85546875" style="53" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="53" customWidth="1"/>
-    <col min="5" max="5" width="37.140625" style="53" customWidth="1"/>
-    <col min="6" max="6" width="40.28515625" style="53" customWidth="1"/>
+    <col min="1" max="1" width="27.453125" style="53" customWidth="1"/>
+    <col min="2" max="3" width="19.81640625" style="53" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" style="53" customWidth="1"/>
+    <col min="5" max="5" width="37.1796875" style="53" customWidth="1"/>
+    <col min="6" max="6" width="40.26953125" style="53" customWidth="1"/>
     <col min="7" max="7" width="29" style="53" customWidth="1"/>
-    <col min="8" max="8" width="54.7109375" style="53" customWidth="1"/>
-    <col min="9" max="10" width="18.42578125" style="53" customWidth="1"/>
+    <col min="8" max="8" width="54.7265625" style="53" customWidth="1"/>
+    <col min="9" max="10" width="18.453125" style="53" customWidth="1"/>
     <col min="11" max="11" width="16" style="53" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" style="53" customWidth="1"/>
+    <col min="12" max="12" width="16.81640625" style="53" customWidth="1"/>
     <col min="13" max="13" width="16" style="53" customWidth="1"/>
     <col min="14" max="15" width="15" style="53" customWidth="1"/>
-    <col min="16" max="16" width="47.140625" style="53" customWidth="1"/>
-    <col min="17" max="17" width="46.28515625" style="53" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="53"/>
+    <col min="16" max="16" width="47.1796875" style="53" customWidth="1"/>
+    <col min="17" max="17" width="46.26953125" style="53" customWidth="1"/>
+    <col min="18" max="16384" width="9.1796875" style="53"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="44" customFormat="1" ht="42" customHeight="1">
       <c r="A1" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="190" t="s">
+      <c r="B1" s="194" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="190"/>
-      <c r="D1" s="191"/>
-      <c r="E1" s="191"/>
-      <c r="F1" s="191"/>
-      <c r="G1" s="191"/>
-      <c r="H1" s="191"/>
-      <c r="I1" s="191"/>
-      <c r="J1" s="191"/>
-      <c r="K1" s="191"/>
-      <c r="L1" s="191"/>
-      <c r="M1" s="191"/>
-      <c r="N1" s="191"/>
-      <c r="O1" s="191"/>
-      <c r="P1" s="191"/>
-      <c r="Q1" s="191"/>
-      <c r="R1" s="191"/>
-      <c r="S1" s="191"/>
-      <c r="T1" s="191"/>
-      <c r="U1" s="191"/>
-      <c r="V1" s="191"/>
-      <c r="W1" s="191"/>
-      <c r="X1" s="191"/>
-      <c r="Y1" s="191"/>
-      <c r="Z1" s="191"/>
-      <c r="AA1" s="191"/>
-      <c r="AB1" s="191"/>
-      <c r="AC1" s="191"/>
+      <c r="C1" s="194"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
+      <c r="F1" s="195"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="195"/>
+      <c r="I1" s="195"/>
+      <c r="J1" s="195"/>
+      <c r="K1" s="195"/>
+      <c r="L1" s="195"/>
+      <c r="M1" s="195"/>
+      <c r="N1" s="195"/>
+      <c r="O1" s="195"/>
+      <c r="P1" s="195"/>
+      <c r="Q1" s="195"/>
+      <c r="R1" s="195"/>
+      <c r="S1" s="195"/>
+      <c r="T1" s="195"/>
+      <c r="U1" s="195"/>
+      <c r="V1" s="195"/>
+      <c r="W1" s="195"/>
+      <c r="X1" s="195"/>
+      <c r="Y1" s="195"/>
+      <c r="Z1" s="195"/>
+      <c r="AA1" s="195"/>
+      <c r="AB1" s="195"/>
+      <c r="AC1" s="195"/>
     </row>
     <row r="2" spans="1:29" s="44" customFormat="1" ht="30.75" customHeight="1">
       <c r="A2" s="45"/>
@@ -8293,7 +8298,7 @@
         <v>30</v>
       </c>
       <c r="K2" s="46" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="L2" s="46" t="s">
         <v>311</v>
@@ -8315,7 +8320,7 @@
       </c>
     </row>
     <row r="3" spans="1:29" ht="123.75" customHeight="1">
-      <c r="A3" s="192" t="s">
+      <c r="A3" s="196" t="s">
         <v>101</v>
       </c>
       <c r="B3" s="47" t="s">
@@ -8350,7 +8355,7 @@
       </c>
       <c r="L3" s="51"/>
       <c r="M3" s="51" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="N3" s="52" t="s">
         <v>109</v>
@@ -8364,7 +8369,7 @@
       </c>
     </row>
     <row r="4" spans="1:29" ht="138.75" customHeight="1">
-      <c r="A4" s="192"/>
+      <c r="A4" s="196"/>
       <c r="B4" s="47" t="s">
         <v>102</v>
       </c>
@@ -8397,7 +8402,7 @@
       </c>
       <c r="L4" s="51"/>
       <c r="M4" s="51" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="N4" s="52" t="s">
         <v>109</v>
@@ -8411,7 +8416,7 @@
       </c>
     </row>
     <row r="5" spans="1:29" ht="124.5" customHeight="1">
-      <c r="A5" s="192"/>
+      <c r="A5" s="196"/>
       <c r="B5" s="47" t="s">
         <v>102</v>
       </c>
@@ -8433,7 +8438,7 @@
       <c r="H5" s="55" t="s">
         <v>125</v>
       </c>
-      <c r="I5" s="193">
+      <c r="I5" s="197">
         <v>2</v>
       </c>
       <c r="J5" s="155">
@@ -8444,7 +8449,7 @@
       </c>
       <c r="L5" s="51"/>
       <c r="M5" s="51" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="N5" s="52" t="s">
         <v>109</v>
@@ -8458,7 +8463,7 @@
       </c>
     </row>
     <row r="6" spans="1:29" ht="64.5" customHeight="1">
-      <c r="A6" s="192"/>
+      <c r="A6" s="196"/>
       <c r="B6" s="47" t="s">
         <v>102</v>
       </c>
@@ -8480,7 +8485,7 @@
       <c r="H6" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="I6" s="193"/>
+      <c r="I6" s="197"/>
       <c r="J6" s="155">
         <v>43984</v>
       </c>
@@ -8489,7 +8494,7 @@
       </c>
       <c r="L6" s="51"/>
       <c r="M6" s="51" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="N6" s="52" t="s">
         <v>109</v>
@@ -8573,26 +8578,26 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="3" width="33.7109375" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" customWidth="1"/>
+    <col min="2" max="3" width="33.7265625" customWidth="1"/>
+    <col min="4" max="4" width="31.7265625" customWidth="1"/>
+    <col min="5" max="5" width="36.7265625" customWidth="1"/>
+    <col min="6" max="6" width="25.453125" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="37.5" customHeight="1">
-      <c r="A1" s="187" t="s">
+      <c r="A1" s="191" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="187"/>
-      <c r="C1" s="187"/>
-      <c r="D1" s="187"/>
-      <c r="E1" s="187"/>
-      <c r="F1" s="187"/>
-      <c r="G1" s="187"/>
+      <c r="B1" s="191"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
+      <c r="E1" s="191"/>
+      <c r="F1" s="191"/>
+      <c r="G1" s="191"/>
     </row>
     <row r="2" spans="1:11" ht="49.5" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -8617,7 +8622,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="75">
+    <row r="3" spans="1:11" ht="72.5">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -8733,106 +8738,106 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" customWidth="1"/>
+    <col min="3" max="3" width="29.1796875" customWidth="1"/>
+    <col min="4" max="4" width="28.81640625" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
-    <col min="6" max="6" width="40.85546875" customWidth="1"/>
-    <col min="7" max="7" width="40.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
-    <col min="10" max="11" width="17.5703125" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="40.81640625" customWidth="1"/>
+    <col min="7" max="7" width="40.1796875" customWidth="1"/>
+    <col min="8" max="8" width="16.1796875" customWidth="1"/>
+    <col min="9" max="9" width="18.1796875" customWidth="1"/>
+    <col min="10" max="11" width="17.54296875" customWidth="1"/>
+    <col min="12" max="12" width="18.54296875" customWidth="1"/>
     <col min="13" max="13" width="24" customWidth="1"/>
-    <col min="14" max="14" width="21.85546875" customWidth="1"/>
-    <col min="15" max="15" width="53.7109375" customWidth="1"/>
-    <col min="16" max="16" width="57.5703125" customWidth="1"/>
+    <col min="14" max="14" width="21.81640625" customWidth="1"/>
+    <col min="15" max="15" width="53.7265625" customWidth="1"/>
+    <col min="16" max="16" width="57.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="176" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="175" t="s">
+      <c r="B1" s="178" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
-      <c r="O1" s="175"/>
-      <c r="P1" s="175"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+      <c r="H1" s="178"/>
+      <c r="I1" s="178"/>
+      <c r="J1" s="178"/>
+      <c r="K1" s="178"/>
+      <c r="L1" s="178"/>
+      <c r="M1" s="178"/>
+      <c r="N1" s="178"/>
+      <c r="O1" s="178"/>
+      <c r="P1" s="178"/>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="174"/>
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
-      <c r="I2" s="175"/>
-      <c r="J2" s="175"/>
-      <c r="K2" s="175"/>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175"/>
-      <c r="N2" s="175"/>
-      <c r="O2" s="175"/>
-      <c r="P2" s="175"/>
+      <c r="A2" s="177"/>
+      <c r="B2" s="178"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="178"/>
+      <c r="I2" s="178"/>
+      <c r="J2" s="178"/>
+      <c r="K2" s="178"/>
+      <c r="L2" s="178"/>
+      <c r="M2" s="178"/>
+      <c r="N2" s="178"/>
+      <c r="O2" s="178"/>
+      <c r="P2" s="178"/>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="174"/>
-      <c r="B3" s="176"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
-      <c r="F3" s="176"/>
-      <c r="G3" s="176"/>
-      <c r="H3" s="176"/>
-      <c r="I3" s="176"/>
-      <c r="J3" s="176"/>
-      <c r="K3" s="176"/>
-      <c r="L3" s="176"/>
-      <c r="M3" s="176"/>
-      <c r="N3" s="176"/>
-      <c r="O3" s="176"/>
-      <c r="P3" s="176"/>
-    </row>
-    <row r="4" spans="1:16" ht="26.25">
+      <c r="A3" s="177"/>
+      <c r="B3" s="179"/>
+      <c r="C3" s="179"/>
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="179"/>
+      <c r="H3" s="179"/>
+      <c r="I3" s="179"/>
+      <c r="J3" s="179"/>
+      <c r="K3" s="179"/>
+      <c r="L3" s="179"/>
+      <c r="M3" s="179"/>
+      <c r="N3" s="179"/>
+      <c r="O3" s="179"/>
+      <c r="P3" s="179"/>
+    </row>
+    <row r="4" spans="1:16" ht="26">
       <c r="A4" s="13"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="177"/>
-      <c r="D4" s="177"/>
-      <c r="E4" s="177"/>
-      <c r="F4" s="177"/>
-      <c r="G4" s="177"/>
-      <c r="H4" s="177"/>
-      <c r="I4" s="177"/>
-      <c r="J4" s="177"/>
-      <c r="K4" s="177"/>
-      <c r="L4" s="177"/>
-      <c r="M4" s="177"/>
-      <c r="N4" s="177"/>
-      <c r="O4" s="177"/>
-      <c r="P4" s="178"/>
-    </row>
-    <row r="5" spans="1:16" ht="60.6" customHeight="1">
+      <c r="B4" s="180"/>
+      <c r="C4" s="180"/>
+      <c r="D4" s="180"/>
+      <c r="E4" s="180"/>
+      <c r="F4" s="180"/>
+      <c r="G4" s="180"/>
+      <c r="H4" s="180"/>
+      <c r="I4" s="180"/>
+      <c r="J4" s="180"/>
+      <c r="K4" s="180"/>
+      <c r="L4" s="180"/>
+      <c r="M4" s="180"/>
+      <c r="N4" s="180"/>
+      <c r="O4" s="180"/>
+      <c r="P4" s="181"/>
+    </row>
+    <row r="5" spans="1:16" ht="60.65" customHeight="1">
       <c r="A5" s="14"/>
       <c r="B5" s="15" t="s">
         <v>23</v>
@@ -8881,7 +8886,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="69.75" customHeight="1">
-      <c r="A6" s="194" t="s">
+      <c r="A6" s="198" t="s">
         <v>60</v>
       </c>
       <c r="B6" s="33" t="s">
@@ -8902,20 +8907,22 @@
       <c r="G6" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="184">
+      <c r="H6" s="187">
         <v>2</v>
       </c>
-      <c r="I6" s="19"/>
+      <c r="I6" s="153">
+        <v>43978</v>
+      </c>
       <c r="J6" s="153">
         <v>43977</v>
       </c>
       <c r="K6" s="36" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="L6" s="154">
         <v>43978</v>
       </c>
-      <c r="M6" s="197" t="s">
+      <c r="M6" s="201" t="s">
         <v>66</v>
       </c>
       <c r="N6" s="37"/>
@@ -8927,7 +8934,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="66.75" customHeight="1">
-      <c r="A7" s="195"/>
+      <c r="A7" s="199"/>
       <c r="B7" s="33" t="s">
         <v>37</v>
       </c>
@@ -8946,18 +8953,20 @@
       <c r="G7" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="H7" s="196"/>
-      <c r="I7" s="19"/>
+      <c r="H7" s="200"/>
+      <c r="I7" s="153">
+        <v>43979</v>
+      </c>
       <c r="J7" s="153">
         <v>43979</v>
       </c>
       <c r="K7" s="36" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="L7" s="154">
         <v>43979</v>
       </c>
-      <c r="M7" s="198"/>
+      <c r="M7" s="202"/>
       <c r="N7" s="37"/>
       <c r="O7" s="38" t="s">
         <v>74</v>
@@ -8996,12 +9005,12 @@
         <v>43980</v>
       </c>
       <c r="K8" s="36" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="L8" s="154">
         <v>43984</v>
       </c>
-      <c r="M8" s="198"/>
+      <c r="M8" s="202"/>
       <c r="N8" s="37"/>
       <c r="O8" s="38" t="s">
         <v>78</v>
@@ -9030,41 +9039,41 @@
   <dimension ref="A1:BZ155"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="30" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" style="29" customWidth="1"/>
-    <col min="4" max="14" width="33.42578125" style="29" customWidth="1"/>
-    <col min="15" max="15" width="61.5703125" style="31" customWidth="1"/>
-    <col min="16" max="16" width="68.7109375" style="12" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="32.7265625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="21.81640625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="30.1796875" style="29" customWidth="1"/>
+    <col min="4" max="14" width="33.453125" style="29" customWidth="1"/>
+    <col min="15" max="15" width="61.54296875" style="31" customWidth="1"/>
+    <col min="16" max="16" width="68.7265625" style="12" customWidth="1"/>
+    <col min="17" max="16384" width="9.1796875" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:78" ht="15" customHeight="1">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="176" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="199" t="s">
+      <c r="B1" s="203" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
-      <c r="E1" s="200"/>
-      <c r="F1" s="200"/>
-      <c r="G1" s="200"/>
-      <c r="H1" s="200"/>
-      <c r="I1" s="200"/>
-      <c r="J1" s="200"/>
-      <c r="K1" s="200"/>
-      <c r="L1" s="200"/>
-      <c r="M1" s="200"/>
-      <c r="N1" s="200"/>
-      <c r="O1" s="200"/>
-      <c r="P1" s="201"/>
+      <c r="C1" s="204"/>
+      <c r="D1" s="204"/>
+      <c r="E1" s="204"/>
+      <c r="F1" s="204"/>
+      <c r="G1" s="204"/>
+      <c r="H1" s="204"/>
+      <c r="I1" s="204"/>
+      <c r="J1" s="204"/>
+      <c r="K1" s="204"/>
+      <c r="L1" s="204"/>
+      <c r="M1" s="204"/>
+      <c r="N1" s="204"/>
+      <c r="O1" s="204"/>
+      <c r="P1" s="205"/>
       <c r="Q1" s="10"/>
       <c r="R1" s="10"/>
       <c r="S1" s="10"/>
@@ -9129,22 +9138,22 @@
       <c r="BZ1" s="11"/>
     </row>
     <row r="2" spans="1:78" ht="15" customHeight="1">
-      <c r="A2" s="174"/>
-      <c r="B2" s="202"/>
-      <c r="C2" s="203"/>
-      <c r="D2" s="203"/>
-      <c r="E2" s="203"/>
-      <c r="F2" s="203"/>
-      <c r="G2" s="203"/>
-      <c r="H2" s="203"/>
-      <c r="I2" s="203"/>
-      <c r="J2" s="203"/>
-      <c r="K2" s="203"/>
-      <c r="L2" s="203"/>
-      <c r="M2" s="203"/>
-      <c r="N2" s="203"/>
-      <c r="O2" s="203"/>
-      <c r="P2" s="204"/>
+      <c r="A2" s="177"/>
+      <c r="B2" s="206"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
+      <c r="E2" s="207"/>
+      <c r="F2" s="207"/>
+      <c r="G2" s="207"/>
+      <c r="H2" s="207"/>
+      <c r="I2" s="207"/>
+      <c r="J2" s="207"/>
+      <c r="K2" s="207"/>
+      <c r="L2" s="207"/>
+      <c r="M2" s="207"/>
+      <c r="N2" s="207"/>
+      <c r="O2" s="207"/>
+      <c r="P2" s="208"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="10"/>
       <c r="S2" s="10"/>
@@ -9209,22 +9218,22 @@
       <c r="BZ2" s="11"/>
     </row>
     <row r="3" spans="1:78" ht="15" customHeight="1">
-      <c r="A3" s="174"/>
-      <c r="B3" s="205"/>
-      <c r="C3" s="206"/>
-      <c r="D3" s="206"/>
-      <c r="E3" s="206"/>
-      <c r="F3" s="206"/>
-      <c r="G3" s="206"/>
-      <c r="H3" s="206"/>
-      <c r="I3" s="206"/>
-      <c r="J3" s="206"/>
-      <c r="K3" s="206"/>
-      <c r="L3" s="206"/>
-      <c r="M3" s="206"/>
-      <c r="N3" s="206"/>
-      <c r="O3" s="206"/>
-      <c r="P3" s="207"/>
+      <c r="A3" s="177"/>
+      <c r="B3" s="209"/>
+      <c r="C3" s="210"/>
+      <c r="D3" s="210"/>
+      <c r="E3" s="210"/>
+      <c r="F3" s="210"/>
+      <c r="G3" s="210"/>
+      <c r="H3" s="210"/>
+      <c r="I3" s="210"/>
+      <c r="J3" s="210"/>
+      <c r="K3" s="210"/>
+      <c r="L3" s="210"/>
+      <c r="M3" s="210"/>
+      <c r="N3" s="210"/>
+      <c r="O3" s="210"/>
+      <c r="P3" s="211"/>
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>
@@ -9288,23 +9297,23 @@
       <c r="BY3" s="11"/>
       <c r="BZ3" s="11"/>
     </row>
-    <row r="4" spans="1:78" ht="26.25">
+    <row r="4" spans="1:78" ht="26">
       <c r="A4" s="13"/>
-      <c r="B4" s="208"/>
-      <c r="C4" s="177"/>
-      <c r="D4" s="177"/>
-      <c r="E4" s="177"/>
-      <c r="F4" s="177"/>
-      <c r="G4" s="177"/>
-      <c r="H4" s="177"/>
-      <c r="I4" s="177"/>
-      <c r="J4" s="177"/>
-      <c r="K4" s="177"/>
-      <c r="L4" s="177"/>
-      <c r="M4" s="177"/>
-      <c r="N4" s="177"/>
-      <c r="O4" s="177"/>
-      <c r="P4" s="178"/>
+      <c r="B4" s="212"/>
+      <c r="C4" s="180"/>
+      <c r="D4" s="180"/>
+      <c r="E4" s="180"/>
+      <c r="F4" s="180"/>
+      <c r="G4" s="180"/>
+      <c r="H4" s="180"/>
+      <c r="I4" s="180"/>
+      <c r="J4" s="180"/>
+      <c r="K4" s="180"/>
+      <c r="L4" s="180"/>
+      <c r="M4" s="180"/>
+      <c r="N4" s="180"/>
+      <c r="O4" s="180"/>
+      <c r="P4" s="181"/>
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
@@ -9478,8 +9487,8 @@
       <c r="BY5" s="11"/>
       <c r="BZ5" s="11"/>
     </row>
-    <row r="6" spans="1:78" ht="90">
-      <c r="A6" s="181" t="s">
+    <row r="6" spans="1:78" ht="87">
+      <c r="A6" s="184" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="18" t="s">
@@ -9511,9 +9520,9 @@
         <v>43979</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>312</v>
-      </c>
-      <c r="M6" s="209" t="s">
+        <v>317</v>
+      </c>
+      <c r="M6" s="213" t="s">
         <v>43</v>
       </c>
       <c r="N6" s="19"/>
@@ -9586,8 +9595,8 @@
       <c r="BY6" s="11"/>
       <c r="BZ6" s="11"/>
     </row>
-    <row r="7" spans="1:78" ht="120">
-      <c r="A7" s="181"/>
+    <row r="7" spans="1:78" ht="116">
+      <c r="A7" s="184"/>
       <c r="B7" s="18" t="s">
         <v>37</v>
       </c>
@@ -9617,9 +9626,9 @@
         <v>43984</v>
       </c>
       <c r="L7" s="25" t="s">
-        <v>312</v>
-      </c>
-      <c r="M7" s="210"/>
+        <v>316</v>
+      </c>
+      <c r="M7" s="214"/>
       <c r="N7" s="19"/>
       <c r="O7" s="22" t="s">
         <v>51</v>
@@ -9690,8 +9699,8 @@
       <c r="BY7" s="11"/>
       <c r="BZ7" s="11"/>
     </row>
-    <row r="8" spans="1:78" ht="120">
-      <c r="A8" s="181"/>
+    <row r="8" spans="1:78" ht="116">
+      <c r="A8" s="184"/>
       <c r="B8" s="18" t="s">
         <v>37</v>
       </c>
@@ -9721,9 +9730,9 @@
         <v>43989</v>
       </c>
       <c r="L8" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="M8" s="210"/>
+        <v>312</v>
+      </c>
+      <c r="M8" s="214"/>
       <c r="N8" s="19"/>
       <c r="O8" s="22" t="s">
         <v>57</v>
@@ -14633,28 +14642,28 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="3" width="33.7109375" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" customWidth="1"/>
+    <col min="2" max="3" width="33.7265625" customWidth="1"/>
+    <col min="4" max="4" width="31.7265625" customWidth="1"/>
+    <col min="5" max="5" width="36.7265625" customWidth="1"/>
+    <col min="6" max="6" width="25.453125" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="187" t="s">
+      <c r="A1" s="191" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="187"/>
-      <c r="C1" s="187"/>
-      <c r="D1" s="187"/>
-      <c r="E1" s="187"/>
-      <c r="F1" s="187"/>
-      <c r="G1" s="187"/>
-    </row>
-    <row r="2" spans="1:11" ht="18.75">
+      <c r="B1" s="191"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
+      <c r="E1" s="191"/>
+      <c r="F1" s="191"/>
+      <c r="G1" s="191"/>
+    </row>
+    <row r="2" spans="1:11" ht="18.5">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -14677,7 +14686,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="45">
+    <row r="3" spans="1:11" ht="43.5">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -14694,7 +14703,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:11" ht="105">
+    <row r="4" spans="1:11" ht="87">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -14713,7 +14722,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:11" ht="105">
+    <row r="5" spans="1:11" ht="87">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -14779,7 +14788,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14792,7 +14801,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14805,7 +14814,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14818,7 +14827,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14831,7 +14840,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="16384" width="10" style="141"/>
   </cols>
@@ -14847,7 +14856,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="16384" width="10" style="141"/>
   </cols>
@@ -14865,28 +14874,28 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="141" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="141" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" style="141" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="141" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" style="141" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" style="141" customWidth="1"/>
+    <col min="3" max="3" width="30.26953125" style="141" customWidth="1"/>
+    <col min="4" max="4" width="23.81640625" style="141" customWidth="1"/>
     <col min="5" max="5" width="21" style="141" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="141" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="141" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" style="141" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" style="141" customWidth="1"/>
     <col min="8" max="16384" width="10" style="141"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33.75" customHeight="1">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="162"/>
-      <c r="G1" s="163"/>
+      <c r="B1" s="165"/>
+      <c r="C1" s="165"/>
+      <c r="D1" s="165"/>
+      <c r="E1" s="165"/>
+      <c r="F1" s="165"/>
+      <c r="G1" s="166"/>
     </row>
     <row r="2" spans="1:7" ht="49.5" customHeight="1">
       <c r="A2" s="142" t="s">
@@ -14926,7 +14935,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45">
+    <row r="4" spans="1:7" ht="29">
       <c r="A4" s="146">
         <v>2</v>
       </c>
@@ -14941,7 +14950,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45">
+    <row r="5" spans="1:7" ht="43.5">
       <c r="A5" s="146">
         <v>3</v>
       </c>
@@ -14956,7 +14965,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30">
+    <row r="6" spans="1:7" ht="29">
       <c r="A6" s="146">
         <v>4</v>
       </c>
@@ -14990,50 +14999,50 @@
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:BZ7"/>
   <sheetViews>
-    <sheetView topLeftCell="F5" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" style="141" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="141" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="141" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="141" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="141" customWidth="1"/>
+    <col min="1" max="1" width="27.453125" style="141" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" style="141" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" style="141" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" style="141" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" style="141" customWidth="1"/>
     <col min="6" max="6" width="16" style="141" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" style="141" customWidth="1"/>
+    <col min="7" max="7" width="28.54296875" style="141" customWidth="1"/>
     <col min="8" max="8" width="10" style="141"/>
-    <col min="9" max="9" width="9.5703125" style="141" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" style="141" customWidth="1"/>
+    <col min="9" max="9" width="9.54296875" style="141" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" style="141" customWidth="1"/>
     <col min="11" max="12" width="10" style="141" customWidth="1"/>
     <col min="13" max="14" width="10" style="141"/>
-    <col min="15" max="15" width="44.7109375" style="141" customWidth="1"/>
-    <col min="16" max="16" width="50.28515625" style="141" customWidth="1"/>
+    <col min="15" max="15" width="44.7265625" style="141" customWidth="1"/>
+    <col min="16" max="16" width="50.26953125" style="141" customWidth="1"/>
     <col min="17" max="16384" width="10" style="141"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:78" s="130" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="164" t="s">
+      <c r="A1" s="167" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="166" t="s">
+      <c r="B1" s="169" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="166"/>
-      <c r="L1" s="166"/>
-      <c r="M1" s="166"/>
-      <c r="N1" s="166"/>
-      <c r="O1" s="166"/>
-      <c r="P1" s="166"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
+      <c r="G1" s="169"/>
+      <c r="H1" s="169"/>
+      <c r="I1" s="169"/>
+      <c r="J1" s="169"/>
+      <c r="K1" s="169"/>
+      <c r="L1" s="169"/>
+      <c r="M1" s="169"/>
+      <c r="N1" s="169"/>
+      <c r="O1" s="169"/>
+      <c r="P1" s="169"/>
       <c r="Q1" s="128"/>
       <c r="R1" s="128"/>
       <c r="S1" s="128"/>
@@ -15098,22 +15107,22 @@
       <c r="BZ1" s="129"/>
     </row>
     <row r="2" spans="1:78" s="130" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="165"/>
-      <c r="B2" s="166"/>
-      <c r="C2" s="166"/>
-      <c r="D2" s="166"/>
-      <c r="E2" s="166"/>
-      <c r="F2" s="166"/>
-      <c r="G2" s="166"/>
-      <c r="H2" s="166"/>
-      <c r="I2" s="166"/>
-      <c r="J2" s="166"/>
-      <c r="K2" s="166"/>
-      <c r="L2" s="166"/>
-      <c r="M2" s="166"/>
-      <c r="N2" s="166"/>
-      <c r="O2" s="166"/>
-      <c r="P2" s="166"/>
+      <c r="A2" s="168"/>
+      <c r="B2" s="169"/>
+      <c r="C2" s="169"/>
+      <c r="D2" s="169"/>
+      <c r="E2" s="169"/>
+      <c r="F2" s="169"/>
+      <c r="G2" s="169"/>
+      <c r="H2" s="169"/>
+      <c r="I2" s="169"/>
+      <c r="J2" s="169"/>
+      <c r="K2" s="169"/>
+      <c r="L2" s="169"/>
+      <c r="M2" s="169"/>
+      <c r="N2" s="169"/>
+      <c r="O2" s="169"/>
+      <c r="P2" s="169"/>
       <c r="Q2" s="128"/>
       <c r="R2" s="128"/>
       <c r="S2" s="128"/>
@@ -15178,22 +15187,22 @@
       <c r="BZ2" s="129"/>
     </row>
     <row r="3" spans="1:78" s="130" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="165"/>
-      <c r="B3" s="167"/>
-      <c r="C3" s="167"/>
-      <c r="D3" s="167"/>
-      <c r="E3" s="167"/>
-      <c r="F3" s="167"/>
-      <c r="G3" s="167"/>
-      <c r="H3" s="167"/>
-      <c r="I3" s="167"/>
-      <c r="J3" s="167"/>
-      <c r="K3" s="167"/>
-      <c r="L3" s="167"/>
-      <c r="M3" s="167"/>
-      <c r="N3" s="167"/>
-      <c r="O3" s="167"/>
-      <c r="P3" s="167"/>
+      <c r="A3" s="168"/>
+      <c r="B3" s="170"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="170"/>
+      <c r="H3" s="170"/>
+      <c r="I3" s="170"/>
+      <c r="J3" s="170"/>
+      <c r="K3" s="170"/>
+      <c r="L3" s="170"/>
+      <c r="M3" s="170"/>
+      <c r="N3" s="170"/>
+      <c r="O3" s="170"/>
+      <c r="P3" s="170"/>
       <c r="Q3" s="128"/>
       <c r="R3" s="128"/>
       <c r="S3" s="128"/>
@@ -15257,23 +15266,23 @@
       <c r="BY3" s="129"/>
       <c r="BZ3" s="129"/>
     </row>
-    <row r="4" spans="1:78" s="130" customFormat="1" ht="26.25">
+    <row r="4" spans="1:78" s="130" customFormat="1" ht="26">
       <c r="A4" s="131"/>
-      <c r="B4" s="168"/>
-      <c r="C4" s="168"/>
-      <c r="D4" s="168"/>
-      <c r="E4" s="168"/>
-      <c r="F4" s="168"/>
-      <c r="G4" s="168"/>
-      <c r="H4" s="168"/>
-      <c r="I4" s="168"/>
-      <c r="J4" s="168"/>
-      <c r="K4" s="168"/>
-      <c r="L4" s="168"/>
-      <c r="M4" s="168"/>
-      <c r="N4" s="168"/>
-      <c r="O4" s="168"/>
-      <c r="P4" s="169"/>
+      <c r="B4" s="171"/>
+      <c r="C4" s="171"/>
+      <c r="D4" s="171"/>
+      <c r="E4" s="171"/>
+      <c r="F4" s="171"/>
+      <c r="G4" s="171"/>
+      <c r="H4" s="171"/>
+      <c r="I4" s="171"/>
+      <c r="J4" s="171"/>
+      <c r="K4" s="171"/>
+      <c r="L4" s="171"/>
+      <c r="M4" s="171"/>
+      <c r="N4" s="171"/>
+      <c r="O4" s="171"/>
+      <c r="P4" s="172"/>
       <c r="Q4" s="128"/>
       <c r="R4" s="128"/>
       <c r="S4" s="128"/>
@@ -15480,7 +15489,7 @@
         <v>43980</v>
       </c>
       <c r="L6" s="138" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="M6" s="137" t="s">
         <v>290</v>
@@ -15588,7 +15597,7 @@
         <v>43984</v>
       </c>
       <c r="L7" s="138" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M7" s="137" t="s">
         <v>290</v>
@@ -15682,27 +15691,27 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.7265625" customWidth="1"/>
+    <col min="4" max="4" width="31.26953125" customWidth="1"/>
+    <col min="5" max="5" width="29.1796875" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33.75" customHeight="1">
-      <c r="A1" s="170" t="s">
+      <c r="A1" s="173" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="171"/>
-      <c r="C1" s="171"/>
-      <c r="D1" s="171"/>
-      <c r="E1" s="171"/>
-      <c r="F1" s="171"/>
-      <c r="G1" s="172"/>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="175"/>
     </row>
     <row r="2" spans="1:7" ht="49.5" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -15742,7 +15751,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="47.1" customHeight="1">
+    <row r="4" spans="1:7" ht="47.15" customHeight="1">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -15757,7 +15766,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45">
+    <row r="5" spans="1:7" ht="43.5">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -15772,7 +15781,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="54.95" customHeight="1">
+    <row r="6" spans="1:7" ht="55" customHeight="1">
       <c r="A6" s="120">
         <v>4</v>
       </c>
@@ -15787,7 +15796,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="51.95" customHeight="1">
+    <row r="7" spans="1:7" ht="52" customHeight="1">
       <c r="A7" s="121">
         <v>5</v>
       </c>

</xml_diff>